<commit_message>
new excel data structure
</commit_message>
<xml_diff>
--- a/data/optimization_config.xlsx
+++ b/data/optimization_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eggy\dissertation-files-final\bioreactor-implementation-june\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E87EB6E0-8383-4D66-891A-91D9D4598C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F365F99F-D698-40F3-98D0-BFEA78FF0FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1439,7 +1439,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1669,6 +1669,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3112,7 +3113,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
analysis python files, plotting, etc.
</commit_message>
<xml_diff>
--- a/data/optimization_config.xlsx
+++ b/data/optimization_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eggy\dissertation-files-final\bioreactor-implementation-june\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eggy\dissertation-files-final\dissertation-cbrem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CDAECB1-A2B6-49B7-88B0-CFFAB183CD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42343C00-5A6D-4041-83FA-6B397DFFCADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
   <si>
     <t>Parameter</t>
   </si>
@@ -265,6 +265,48 @@
   </si>
   <si>
     <t>Wastage flow [m3/d]</t>
+  </si>
+  <si>
+    <t>inf_BOD</t>
+  </si>
+  <si>
+    <t>inf_COD</t>
+  </si>
+  <si>
+    <t>inf_TKN</t>
+  </si>
+  <si>
+    <t>inf_TN</t>
+  </si>
+  <si>
+    <t>inf_TP</t>
+  </si>
+  <si>
+    <t>inf_TSS</t>
+  </si>
+  <si>
+    <t>inf_VSS</t>
+  </si>
+  <si>
+    <t>Raw Influent Biological Oxygen Demand (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Chemical Oxygen Demand (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Total Kjedhal Nitrogen (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Total Nitrogen (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Total Phosphorus (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Total Suspended Solids (mg/L)</t>
+  </si>
+  <si>
+    <t>Raw Influent Volatile Suspended Solids (mg/L)</t>
   </si>
 </sst>
 </file>
@@ -669,10 +711,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -888,6 +930,83 @@
       </c>
       <c r="C19" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20">
+        <v>379.82797943309998</v>
+      </c>
+      <c r="C20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21">
+        <v>1760.4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
+      <c r="B22">
+        <v>154.42099999999999</v>
+      </c>
+      <c r="C22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23">
+        <v>174.42099999999999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24">
+        <v>166.740350277819</v>
+      </c>
+      <c r="C24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25">
+        <v>1182.6926908329499</v>
+      </c>
+      <c r="C25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <v>771.45741272220005</v>
+      </c>
+      <c r="C26" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -987,7 +1106,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1071,7 +1190,7 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <v>500</v>
@@ -1132,7 +1251,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD7"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Optuna incorporation into training
</commit_message>
<xml_diff>
--- a/data/optimization_config.xlsx
+++ b/data/optimization_config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eggy\dissertation-files-final\dissertation-cbrem\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{549C6055-8CB1-4D25-97C4-0817B70CFD00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3049843E-8ECF-4A86-B2A3-B67AA221ED07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="91">
   <si>
     <t>Parameter</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Target_Effluent_TP (mg/L)</t>
   </si>
   <si>
-    <t>Target_Effluent_TSS (mg/L)</t>
-  </si>
-  <si>
     <t>Path to the trained CSTR surrogate model.</t>
   </si>
   <si>
@@ -307,6 +304,12 @@
   </si>
   <si>
     <t>Raw Influent Volatile Suspended Solids (mg/L)</t>
+  </si>
+  <si>
+    <t>Target_Effluent_TN (mg/L)</t>
+  </si>
+  <si>
+    <t>Target_Effluent_TKN (mg/L)</t>
   </si>
 </sst>
 </file>
@@ -681,13 +684,13 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -695,13 +698,13 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -736,277 +739,277 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3">
         <v>1000</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B5">
         <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6">
         <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>120</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
         <v>0.5</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11">
         <v>62</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12">
         <v>86</v>
       </c>
       <c r="C12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13">
         <v>0.1</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B14">
         <v>0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15">
         <v>0.1</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16">
         <v>0.1</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19">
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B20">
         <v>379.82797943309998</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B21">
         <v>1760.4</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B22">
         <v>154.42099999999999</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B23">
         <v>174.42099999999999</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B24">
         <v>166.740350277819</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25">
         <v>1182.6926908329499</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26">
         <v>771.45741272220005</v>
       </c>
       <c r="C26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1069,7 +1072,7 @@
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -1077,7 +1080,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -1085,7 +1088,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -1093,7 +1096,7 @@
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1109,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1140,7 +1143,7 @@
         <v>10000</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -1154,7 +1157,7 @@
         <v>10000</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -1168,7 +1171,7 @@
         <v>10000</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -1182,7 +1185,7 @@
         <v>4000</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -1190,13 +1193,13 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="C6">
         <v>500</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -1210,7 +1213,7 @@
         <v>2500</v>
       </c>
       <c r="D7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -1224,7 +1227,7 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -1238,7 +1241,7 @@
         <v>10000</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1248,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1275,10 +1278,10 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1286,7 +1289,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>100</v>
@@ -1297,7 +1300,7 @@
         <v>24</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -1305,13 +1308,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="B5">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>200</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>